<commit_message>
added scenarios and activity-diagrams to section user requirements
</commit_message>
<xml_diff>
--- a/doc/task04/uc-1_Dashboard/uc1_scenario.xlsx
+++ b/doc/task04/uc-1_Dashboard/uc1_scenario.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13035"/>
+    <workbookView windowWidth="20490" windowHeight="8745"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -130,11 +130,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,50 +144,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -201,6 +188,81 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -209,11 +271,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -224,81 +292,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -327,181 +320,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,15 +532,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -563,17 +547,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -602,13 +591,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -617,145 +610,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -766,17 +759,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1094,14 +1087,15 @@
   <sheetPr/>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="3"/>
   <cols>
-    <col min="3" max="3" width="10.8" customWidth="1"/>
-    <col min="4" max="4" width="51.4" customWidth="1"/>
+    <col min="2" max="2" width="8.31333333333333" customWidth="1"/>
+    <col min="3" max="3" width="20.7" customWidth="1"/>
+    <col min="4" max="4" width="50.7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1349,6 +1343,7 @@
     <mergeCell ref="B7:C7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" orientation="landscape"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>